<commit_message>
调整jar包使JSP页面上能直接使用EL. Standard 1.1.jar JSTL 1.1.jar Servlet 2.4, JavaServer Pages 2.0
</commit_message>
<xml_diff>
--- a/trunk/工作计划安排.xlsx
+++ b/trunk/工作计划安排.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="20111221" sheetId="1" r:id="rId1"/>
     <sheet name="20111222" sheetId="2" r:id="rId2"/>
     <sheet name="20111223" sheetId="3" r:id="rId3"/>
     <sheet name="20111226" sheetId="4" r:id="rId4"/>
+    <sheet name="20111227" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t>1、</t>
   </si>
@@ -206,6 +207,15 @@
   </si>
   <si>
     <t>页面返回问题</t>
+  </si>
+  <si>
+    <t>22:20-23:20</t>
+  </si>
+  <si>
+    <t>完成修改和删除功能</t>
+  </si>
+  <si>
+    <t>9:30-11:30</t>
   </si>
 </sst>
 </file>
@@ -832,10 +842,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="H10:M30"/>
+  <dimension ref="H10:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -929,40 +939,40 @@
       </c>
     </row>
     <row r="19" spans="8:13">
-      <c r="H19" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" t="s">
-        <v>60</v>
+      <c r="K19" t="s">
+        <v>63</v>
+      </c>
+      <c r="M19" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="8:13">
       <c r="H20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="8:13">
       <c r="H21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="8:13">
+      <c r="H22" t="s">
         <v>49</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I22" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="8:13">
-      <c r="I24" t="s">
-        <v>2</v>
-      </c>
-      <c r="K24" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="25" spans="8:13">
       <c r="I25" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="K25" t="s">
         <v>57</v>
@@ -970,25 +980,62 @@
     </row>
     <row r="26" spans="8:13">
       <c r="I26" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="K26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="8:13">
       <c r="I27" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="8:13">
       <c r="I28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="8:13">
+      <c r="I29" t="s">
         <v>6</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="8:13">
-      <c r="J30" t="s">
+    <row r="31" spans="8:13">
+      <c r="J31" t="s">
         <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="H9:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="9" spans="8:14">
+      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>